<commit_message>
Revert "Revert "Revert "dfe"""
This reverts commit 4527e5abe7367027863d3561e548aff9feaaf2f1.
</commit_message>
<xml_diff>
--- a/英雄背包，队伍，仓库，强化分解视图.xlsx
+++ b/英雄背包，队伍，仓库，强化分解视图.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="6340" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
   <si>
     <t>英雄分类界面</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -265,10 +265,6 @@
   </si>
   <si>
     <t>MaterialInmationView</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nami</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -646,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -908,11 +904,6 @@
       </c>
       <c r="C38" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="C40" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>